<commit_message>
Added some notes and parts spreadsheets
git-svn-id: http://www.audionest.org/svn/private/audiowidget@130 12d19c19-674d-4888-9b15-31778f81bca0
</commit_message>
<xml_diff>
--- a/notes/da_platform_interfaces_v2.xlsx
+++ b/notes/da_platform_interfaces_v2.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cdp\notes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -16,17 +11,12 @@
     <sheet name="budget" sheetId="3" r:id="rId2"/>
     <sheet name="parts" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="114210"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="171">
   <si>
     <t>Rpi/FPGA to iso</t>
   </si>
@@ -544,8 +534,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,18 +546,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -579,19 +567,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor indexed="13"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor indexed="27"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor indexed="47"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -711,14 +699,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -765,7 +745,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -800,7 +780,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -977,27 +957,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:Q87"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="24" customWidth="1"/>
     <col min="3" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15">
       <c r="B2" s="6" t="s">
         <v>59</v>
       </c>
@@ -1007,7 +987,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15">
       <c r="B3" s="9" t="s">
         <v>60</v>
       </c>
@@ -1016,7 +996,7 @@
       </c>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15">
       <c r="B4" s="9" t="s">
         <v>61</v>
       </c>
@@ -1025,7 +1005,7 @@
       </c>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15">
       <c r="B5" s="13" t="s">
         <v>62</v>
       </c>
@@ -1034,7 +1014,7 @@
       </c>
       <c r="D5" s="15"/>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15">
       <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1031,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15">
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -1068,7 +1048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15">
       <c r="B9" t="s">
         <v>116</v>
       </c>
@@ -1085,7 +1065,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1082,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15">
       <c r="B11" t="s">
         <v>37</v>
       </c>
@@ -1119,7 +1099,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15">
       <c r="B12" t="s">
         <v>5</v>
       </c>
@@ -1136,7 +1116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15">
       <c r="B13" t="s">
         <v>34</v>
       </c>
@@ -1153,7 +1133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -1170,7 +1150,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15">
       <c r="B15" t="s">
         <v>12</v>
       </c>
@@ -1187,7 +1167,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15">
       <c r="B16" t="s">
         <v>13</v>
       </c>
@@ -1204,7 +1184,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1221,7 +1201,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17">
       <c r="B18" t="s">
         <v>18</v>
       </c>
@@ -1238,7 +1218,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17">
       <c r="B19" t="s">
         <v>20</v>
       </c>
@@ -1258,7 +1238,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -1275,7 +1255,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17">
       <c r="B21" t="s">
         <v>25</v>
       </c>
@@ -1292,7 +1272,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -1309,7 +1289,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17">
       <c r="B23" t="s">
         <v>40</v>
       </c>
@@ -1326,12 +1306,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17">
       <c r="N24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17">
       <c r="B25" t="s">
         <v>35</v>
       </c>
@@ -1351,7 +1331,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17">
       <c r="B26" t="s">
         <v>36</v>
       </c>
@@ -1360,7 +1340,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17">
       <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
@@ -1368,7 +1348,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17">
       <c r="B29" t="s">
         <v>5</v>
       </c>
@@ -1376,7 +1356,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17">
       <c r="B30" t="s">
         <v>56</v>
       </c>
@@ -1390,7 +1370,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17">
       <c r="B31" t="s">
         <v>57</v>
       </c>
@@ -1401,7 +1381,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17">
       <c r="B32" t="s">
         <v>64</v>
       </c>
@@ -1409,7 +1389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8">
       <c r="B33" t="s">
         <v>65</v>
       </c>
@@ -1417,7 +1397,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8">
       <c r="B35" s="2" t="s">
         <v>66</v>
       </c>
@@ -1425,7 +1405,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8">
       <c r="B36" t="s">
         <v>5</v>
       </c>
@@ -1436,7 +1416,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8">
       <c r="B37" t="s">
         <v>67</v>
       </c>
@@ -1447,7 +1427,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8">
       <c r="B38" t="s">
         <v>68</v>
       </c>
@@ -1455,7 +1435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8">
       <c r="B39" t="s">
         <v>69</v>
       </c>
@@ -1466,7 +1446,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8">
       <c r="B40" t="s">
         <v>70</v>
       </c>
@@ -1474,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8">
       <c r="B41" t="s">
         <v>71</v>
       </c>
@@ -1482,7 +1462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8">
       <c r="B42" t="s">
         <v>72</v>
       </c>
@@ -1490,12 +1470,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8">
       <c r="B44" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8">
       <c r="B45" t="s">
         <v>79</v>
       </c>
@@ -1503,22 +1483,22 @@
         <v>124</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8">
       <c r="B46" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8">
       <c r="B47" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8">
       <c r="B48" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8">
       <c r="B49" t="s">
         <v>83</v>
       </c>
@@ -1526,22 +1506,22 @@
         <v>99</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8">
       <c r="B50" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8">
       <c r="B51" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8">
       <c r="B53" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8">
       <c r="B54" t="s">
         <v>117</v>
       </c>
@@ -1552,7 +1532,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8">
       <c r="B55" t="s">
         <v>92</v>
       </c>
@@ -1563,7 +1543,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8">
       <c r="B56" t="s">
         <v>93</v>
       </c>
@@ -1574,7 +1554,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8">
       <c r="B57" t="s">
         <v>94</v>
       </c>
@@ -1585,7 +1565,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8">
       <c r="B58" t="s">
         <v>116</v>
       </c>
@@ -1596,7 +1576,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8">
       <c r="B59" t="s">
         <v>7</v>
       </c>
@@ -1607,229 +1587,241 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8">
       <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60">
+        <v>1</v>
+      </c>
+      <c r="G60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8">
+      <c r="B61" t="s">
         <v>34</v>
       </c>
-      <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="G60" t="s">
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="G61" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="62" spans="2:8">
+      <c r="B62" t="s">
         <v>18</v>
       </c>
-      <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="G61" t="s">
+      <c r="E62">
+        <v>1</v>
+      </c>
+      <c r="G62" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="63" spans="2:8">
+      <c r="B63" t="s">
         <v>20</v>
       </c>
-      <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="G62" t="s">
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="G63" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="64" spans="2:8">
+      <c r="B64" t="s">
         <v>22</v>
       </c>
-      <c r="D63">
-        <v>1</v>
-      </c>
-      <c r="G63" t="s">
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="G64" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="65" spans="2:7">
+      <c r="B65" t="s">
         <v>39</v>
       </c>
-      <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="G64" t="s">
+      <c r="E65">
+        <v>1</v>
+      </c>
+      <c r="G65" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="66" spans="2:7">
+      <c r="B66" t="s">
         <v>40</v>
       </c>
-      <c r="D65">
-        <v>1</v>
-      </c>
-      <c r="G65" t="s">
+      <c r="D66">
+        <v>1</v>
+      </c>
+      <c r="G66" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="67" spans="2:7">
+      <c r="B67" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="68" spans="2:7">
+      <c r="B68" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+    <row r="69" spans="2:7">
+      <c r="B69" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+    <row r="70" spans="2:7">
+      <c r="B70" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+    <row r="71" spans="2:7">
+      <c r="B71" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+    <row r="72" spans="2:7">
+      <c r="B72" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+    <row r="73" spans="2:7">
+      <c r="B73" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+    <row r="74" spans="2:7">
+      <c r="B74" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+    <row r="75" spans="2:7">
+      <c r="B75" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+    <row r="76" spans="2:7">
+      <c r="B76" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="77" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B77" s="2" t="s">
+    <row r="78" spans="2:7">
+      <c r="B78" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+    <row r="79" spans="2:7">
+      <c r="B79" t="s">
         <v>118</v>
-      </c>
-      <c r="D78">
-        <v>2</v>
-      </c>
-      <c r="G78" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="79" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>119</v>
       </c>
       <c r="D79">
         <v>2</v>
       </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7">
       <c r="B80" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D80">
         <v>2</v>
       </c>
-      <c r="J80" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="81" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="2:10">
       <c r="B81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D81">
         <v>2</v>
       </c>
       <c r="J81" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="82" spans="2:10" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="2:10">
       <c r="B82" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D82">
         <v>2</v>
       </c>
-      <c r="G82" t="s">
+      <c r="J82" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="83" spans="2:10">
+      <c r="B83" t="s">
+        <v>122</v>
+      </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="G83" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="83" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+    <row r="84" spans="2:10">
+      <c r="B84" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="84" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+    <row r="85" spans="2:10">
+      <c r="B85" t="s">
         <v>104</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J85" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+    <row r="86" spans="2:10">
+      <c r="B86" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="86" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>1</v>
-      </c>
-      <c r="E86">
-        <v>1</v>
-      </c>
-      <c r="G86" t="s">
+    <row r="87" spans="2:10">
+      <c r="B87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+      <c r="G87" t="s">
         <v>123</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9">
       <c r="D1" s="1" t="s">
         <v>164</v>
       </c>
@@ -1837,7 +1829,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9">
       <c r="B2" s="2" t="s">
         <v>145</v>
       </c>
@@ -1857,7 +1849,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>147</v>
       </c>
@@ -1879,7 +1871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>148</v>
       </c>
@@ -1901,7 +1893,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>149</v>
       </c>
@@ -1920,7 +1912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>158</v>
       </c>
@@ -1939,7 +1931,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>159</v>
       </c>
@@ -1958,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>150</v>
       </c>
@@ -1977,7 +1969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>151</v>
       </c>
@@ -1996,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>152</v>
       </c>
@@ -2015,7 +2007,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>153</v>
       </c>
@@ -2031,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>154</v>
       </c>
@@ -2050,7 +2042,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>155</v>
       </c>
@@ -2069,7 +2061,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9">
       <c r="B14" t="s">
         <v>156</v>
       </c>
@@ -2092,7 +2084,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9">
       <c r="B15" t="s">
         <v>157</v>
       </c>
@@ -2111,7 +2103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9">
       <c r="B16" t="s">
         <v>163</v>
       </c>
@@ -2133,7 +2125,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9">
       <c r="B17" t="s">
         <v>160</v>
       </c>
@@ -2152,7 +2144,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9">
       <c r="B18" t="s">
         <v>162</v>
       </c>
@@ -2171,7 +2163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9">
       <c r="B19" t="s">
         <v>161</v>
       </c>
@@ -2193,7 +2185,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9">
       <c r="B20" t="s">
         <v>169</v>
       </c>
@@ -2215,7 +2207,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9">
       <c r="B21" t="s">
         <v>170</v>
       </c>
@@ -2233,11 +2225,11 @@
         <v>40</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21" si="2">C21*E21</f>
+        <f>C21*E21</f>
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9">
       <c r="B28" t="s">
         <v>167</v>
       </c>
@@ -2251,31 +2243,32 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.42578125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>128</v>
       </c>
@@ -2292,7 +2285,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>133</v>
       </c>
@@ -2309,7 +2302,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>136</v>
       </c>
@@ -2323,7 +2316,7 @@
         <v>20.22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -2331,7 +2324,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -2346,6 +2339,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>